<commit_message>
Catalogos base para SAT
</commit_message>
<xml_diff>
--- a/Facturacion Electronica/SAT/Catalogos/CATALOGOS SAT.xlsx
+++ b/Facturacion Electronica/SAT/Catalogos/CATALOGOS SAT.xlsx
@@ -5,31 +5,40 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.vazquez\Documents\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar.hernandez\Documents\GitHub\Projects\Facturacion Electronica\SAT\Catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEEED52D-390B-4E7E-9F58-B85DB6013D5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455C443B-AE87-4D77-9C28-BF5639CB717F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8760" xr2:uid="{1D319FDE-6014-4894-B745-6EACF79A35F5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8760" activeTab="1" xr2:uid="{1D319FDE-6014-4894-B745-6EACF79A35F5}"/>
   </bookViews>
   <sheets>
     <sheet name="CVE PROD SERV" sheetId="1" r:id="rId1"/>
-    <sheet name="FORMA PAGO" sheetId="2" r:id="rId2"/>
-    <sheet name="CLAVE UNIDAD" sheetId="3" r:id="rId3"/>
-    <sheet name="USO CFDI" sheetId="4" r:id="rId4"/>
-    <sheet name="METODO PAGO" sheetId="5" r:id="rId5"/>
+    <sheet name="Hoja1" sheetId="6" r:id="rId2"/>
+    <sheet name="FORMA PAGO" sheetId="2" r:id="rId3"/>
+    <sheet name="CLAVE UNIDAD" sheetId="3" r:id="rId4"/>
+    <sheet name="USO CFDI" sheetId="4" r:id="rId5"/>
+    <sheet name="METODO PAGO" sheetId="5" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CVE PROD SERV'!$A$1:$E$77</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="236">
   <si>
     <t>UTILLAJE</t>
   </si>
@@ -337,9 +346,6 @@
     <t>MAQUINAS DUPLICADORAS</t>
   </si>
   <si>
-    <t>BRASS PLASTIC HEAD KEYS MARQUISTAS</t>
-  </si>
-  <si>
     <t>VA0PAQ</t>
   </si>
   <si>
@@ -379,21 +385,12 @@
     <t>JM0TPA</t>
   </si>
   <si>
-    <t>STEEL KEYS WITH TRANSPONDER</t>
-  </si>
-  <si>
     <t>JM0TPL</t>
   </si>
   <si>
-    <t>BRASS KEYS WITH TRANSPONDER</t>
-  </si>
-  <si>
     <t>JM0TPP</t>
   </si>
   <si>
-    <t>NIKEL KEYS WITH TRANSPONDER</t>
-  </si>
-  <si>
     <t>LLAVES DE CABEZA PLASTICO, ACERO</t>
   </si>
   <si>
@@ -734,12 +731,30 @@
   </si>
   <si>
     <t>PAGO EN PARCIALIDADES O DIFERIDO</t>
+  </si>
+  <si>
+    <t>IFAM CILINDROS SERIE  D</t>
+  </si>
+  <si>
+    <t>IFAM CILINDROS SERIE  M</t>
+  </si>
+  <si>
+    <t>ACCESORIOS DE MAQUINAS DUPLICADORAS</t>
+  </si>
+  <si>
+    <t>PZA</t>
+  </si>
+  <si>
+    <t>ALTUNA\AR.HERNANDEZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -783,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -791,6 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1105,9 +1121,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3C037F-80DC-4A4C-8835-E64848FE7987}">
-  <dimension ref="A1:H175"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" activeCellId="3" sqref="A1 C1 D1 E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1119,28 +1138,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>44101500</v>
       </c>
@@ -1148,20 +1167,20 @@
         <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" t="str">
-        <f>VLOOKUP(B2,G$2:H$175,2,FALSE)</f>
-        <v>MD0990</v>
+        <v>164</v>
+      </c>
+      <c r="D2" t="e">
+        <f t="shared" ref="D2:D33" si="0">VLOOKUP(B2,G$2:H$175,2,FALSE)</f>
+        <v>#N/A</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1172,68 +1191,68 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D3" t="str">
-        <f>VLOOKUP(B3,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>FR0000</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="H3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>46171500</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D4" t="e">
-        <f>VLOOKUP(B4,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>46171500</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D5" t="e">
-        <f>VLOOKUP(B5,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="H5" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1244,20 +1263,20 @@
         <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D6" t="str">
-        <f>VLOOKUP(B6,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0CSF</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1268,20 +1287,20 @@
         <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D7" t="str">
-        <f>VLOOKUP(B7,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0SB0</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1292,20 +1311,20 @@
         <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D8" t="str">
-        <f>VLOOKUP(B8,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0SE0</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1316,20 +1335,20 @@
         <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D9" t="str">
-        <f>VLOOKUP(B9,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0SJ0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1340,23 +1359,23 @@
         <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D10" t="str">
-        <f>VLOOKUP(B10,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0ZC0</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>46171500</v>
       </c>
@@ -1364,23 +1383,23 @@
         <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
-      </c>
-      <c r="D11" t="str">
-        <f>VLOOKUP(B11,G$2:H$175,2,FALSE)</f>
-        <v>IF0ZD0</v>
+        <v>164</v>
+      </c>
+      <c r="D11" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>46171500</v>
       </c>
@@ -1388,20 +1407,20 @@
         <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
-      </c>
-      <c r="D12" t="str">
-        <f>VLOOKUP(B12,G$2:H$175,2,FALSE)</f>
-        <v>IF0ZM0</v>
+        <v>164</v>
+      </c>
+      <c r="D12" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1412,20 +1431,20 @@
         <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D13" t="str">
-        <f>VLOOKUP(B13,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0ZRX</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,92 +1455,92 @@
         <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D14" t="str">
-        <f>VLOOKUP(B14,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0ZWX</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>46171500</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D15" t="e">
-        <f>VLOOKUP(B15,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>46171500</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D16" t="e">
-        <f>VLOOKUP(B16,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>46171500</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D17" t="e">
-        <f>VLOOKUP(B17,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1532,20 +1551,20 @@
         <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D18" t="str">
-        <f>VLOOKUP(B18,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0CDC</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G18" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1556,20 +1575,20 @@
         <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D19" t="str">
-        <f>VLOOKUP(B19,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0CK0</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="H19" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1580,20 +1599,20 @@
         <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D20" t="str">
-        <f>VLOOKUP(B20,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0CS0</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="H20" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1604,20 +1623,20 @@
         <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D21" t="str">
-        <f>VLOOKUP(B21,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0CT0</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G21" t="s">
-        <v>32</v>
+        <v>231</v>
       </c>
       <c r="H21" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1628,20 +1647,20 @@
         <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D22" t="str">
-        <f>VLOOKUP(B22,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0CX0</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>232</v>
       </c>
       <c r="H22" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1652,20 +1671,20 @@
         <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D23" t="str">
-        <f>VLOOKUP(B23,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>IF0CZ0</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1676,20 +1695,20 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D24" t="str">
-        <f>VLOOKUP(B24,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>JM0A00</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="H24" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1700,20 +1719,20 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D25" t="str">
-        <f>VLOOKUP(B25,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>JM0AC0</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1724,20 +1743,20 @@
         <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D26" t="str">
-        <f>VLOOKUP(B26,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>JM0L00</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="H26" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1748,44 +1767,44 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D27" t="str">
-        <f>VLOOKUP(B27,G$2:H$175,2,FALSE)</f>
-        <v>JM0AN0</v>
+        <f t="shared" si="0"/>
+        <v>JM0PN0</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G27" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="H27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>46171505</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C28" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D28" t="e">
-        <f>VLOOKUP(B28,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="H28" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1796,20 +1815,20 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D29" t="str">
-        <f>VLOOKUP(B29,G$2:H$175,2,FALSE)</f>
-        <v>JM0AP0</v>
+        <f t="shared" si="0"/>
+        <v>JM0PP0</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G29" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="H29" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1820,20 +1839,20 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D30" t="str">
-        <f>VLOOKUP(B30,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>JM0P00</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G30" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1844,20 +1863,20 @@
         <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D31" t="str">
-        <f>VLOOKUP(B31,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>JM0LCM</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G31" t="s">
         <v>16</v>
       </c>
       <c r="H31" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1868,20 +1887,20 @@
         <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D32" t="str">
-        <f>VLOOKUP(B32,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>JM0N00</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G32" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H32" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1892,20 +1911,20 @@
         <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D33" t="str">
-        <f>VLOOKUP(B33,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>JM0GL0</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G33" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1916,20 +1935,20 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D34" t="str">
-        <f>VLOOKUP(B34,G$2:H$175,2,FALSE)</f>
+        <f t="shared" ref="D34:D65" si="1">VLOOKUP(B34,G$2:H$175,2,FALSE)</f>
         <v>JM0T00</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G34" t="s">
-        <v>34</v>
+        <v>120</v>
       </c>
       <c r="H34" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1940,20 +1959,20 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D35" t="str">
-        <f>VLOOKUP(B35,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>JM0X00</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G35" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="H35" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1964,20 +1983,20 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D36" t="str">
-        <f>VLOOKUP(B36,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>JM0TP0</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>122</v>
       </c>
       <c r="H36" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1988,188 +2007,188 @@
         <v>20</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D37" t="str">
-        <f>VLOOKUP(B37,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>JM0LF0</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G37" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="H37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>46171505</v>
       </c>
       <c r="B38" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C38" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D38" t="e">
-        <f>VLOOKUP(B38,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G38" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="H38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>46171505</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C39" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D39" t="e">
-        <f>VLOOKUP(B39,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G39" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="H39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>46171505</v>
       </c>
       <c r="B40" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C40" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D40" t="e">
-        <f>VLOOKUP(B40,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G40" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>46171505</v>
       </c>
       <c r="B41" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D41" t="e">
-        <f>VLOOKUP(B41,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G41" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>46171505</v>
       </c>
       <c r="B42" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C42" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D42" t="e">
-        <f>VLOOKUP(B42,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G42" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="H42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>46171505</v>
       </c>
       <c r="B43" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C43" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D43" t="e">
-        <f>VLOOKUP(B43,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G43" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="H43" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>46171505</v>
       </c>
       <c r="B44" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C44" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D44" t="e">
-        <f>VLOOKUP(B44,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G44" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="H44" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2180,44 +2199,44 @@
         <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D45" t="str">
-        <f>VLOOKUP(B45,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>IF0LI0</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G45" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="H45" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46171505</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C46" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D46" t="e">
-        <f>VLOOKUP(B46,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G46" t="s">
-        <v>75</v>
+        <v>132</v>
       </c>
       <c r="H46" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2228,20 +2247,20 @@
         <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D47" t="str">
-        <f>VLOOKUP(B47,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>IF0BM0</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G47" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="H47" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2252,20 +2271,20 @@
         <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D48" t="str">
-        <f>VLOOKUP(B48,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>JT0TEL</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G48" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="H48" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2276,92 +2295,92 @@
         <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D49" t="str">
-        <f>VLOOKUP(B49,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>TP0000</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G49" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="H49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>31261501</v>
       </c>
       <c r="B50" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C50" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D50" t="e">
-        <f>VLOOKUP(B50,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G50" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="H50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>31261501</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C51" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D51" t="e">
-        <f>VLOOKUP(B51,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G51" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="H51" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>31261501</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D52" t="e">
-        <f>VLOOKUP(B52,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G52" t="s">
-        <v>87</v>
+        <v>233</v>
       </c>
       <c r="H52" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2372,20 +2391,20 @@
         <v>42</v>
       </c>
       <c r="C53" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D53" t="str">
-        <f>VLOOKUP(B53,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>KS0B00</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G53" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="H53" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2396,20 +2415,20 @@
         <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D54" t="str">
-        <f>VLOOKUP(B54,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>KS0K00</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G54" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="H54" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2420,20 +2439,20 @@
         <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D55" t="str">
-        <f>VLOOKUP(B55,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>MD0MD0</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G55" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="H55" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2444,188 +2463,188 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D56" t="str">
-        <f>VLOOKUP(B56,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>PU0000</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G56" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="H56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>11191600</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C57" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D57" t="e">
-        <f>VLOOKUP(B57,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G57" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="H57" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>11191600</v>
       </c>
       <c r="B58" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C58" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D58" t="e">
-        <f>VLOOKUP(B58,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G58" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
       <c r="H58" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>11191600</v>
       </c>
       <c r="B59" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C59" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D59" t="e">
-        <f>VLOOKUP(B59,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G59" t="s">
-        <v>6</v>
+        <v>126</v>
       </c>
       <c r="H59" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>11191600</v>
       </c>
       <c r="B60" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C60" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D60" t="e">
-        <f>VLOOKUP(B60,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G60" t="s">
-        <v>8</v>
+        <v>127</v>
       </c>
       <c r="H60" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>11191602</v>
       </c>
       <c r="B61" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C61" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D61" t="e">
-        <f>VLOOKUP(B61,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G61" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="H61" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>11191610</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C62" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D62" t="e">
-        <f>VLOOKUP(B62,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G62" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="H62" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>11191610</v>
       </c>
       <c r="B63" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C63" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D63" t="e">
-        <f>VLOOKUP(B63,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G63" t="s">
-        <v>14</v>
+        <v>129</v>
       </c>
       <c r="H63" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2633,1119 +2652,1190 @@
         <v>44101500</v>
       </c>
       <c r="B64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D64" t="str">
-        <f>VLOOKUP(B64,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>VA0PAQ</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G64" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="H64" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>44101500</v>
       </c>
       <c r="B65" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D65" t="e">
-        <f>VLOOKUP(B65,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G65" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="H65" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>82101500</v>
       </c>
       <c r="B66" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C66" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D66" t="e">
-        <f>VLOOKUP(B66,G$2:H$175,2,FALSE)</f>
+        <f t="shared" ref="D66:D77" si="2">VLOOKUP(B66,G$2:H$175,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G66" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H66" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>82101500</v>
       </c>
       <c r="B67" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C67" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D67" t="e">
-        <f>VLOOKUP(B67,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G67" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="H67" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>82101500</v>
       </c>
       <c r="B68" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C68" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D68" t="e">
-        <f>VLOOKUP(B68,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G68" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="H68" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>82101500</v>
       </c>
       <c r="B69" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C69" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D69" t="e">
-        <f>VLOOKUP(B69,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G69" t="s">
-        <v>12</v>
-      </c>
-      <c r="H69" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>82101500</v>
       </c>
       <c r="B70" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C70" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D70" t="e">
-        <f>VLOOKUP(B70,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G70" t="s">
-        <v>25</v>
-      </c>
-      <c r="H70" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>82101500</v>
       </c>
       <c r="B71" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C71" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D71" t="e">
-        <f>VLOOKUP(B71,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G71" t="s">
-        <v>27</v>
-      </c>
-      <c r="H71" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>82101500</v>
       </c>
       <c r="B72" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D72" t="e">
-        <f>VLOOKUP(B72,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G72" t="s">
-        <v>8</v>
-      </c>
-      <c r="H72" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>82101500</v>
       </c>
       <c r="B73" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C73" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D73" t="e">
-        <f>VLOOKUP(B73,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G73" t="s">
-        <v>10</v>
-      </c>
-      <c r="H73" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>44101500</v>
       </c>
       <c r="B74" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D74" t="e">
-        <f>VLOOKUP(B74,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="G74" t="s">
-        <v>12</v>
-      </c>
-      <c r="H74" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>78141504</v>
       </c>
       <c r="B75" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C75" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D75" t="e">
-        <f>VLOOKUP(B75,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G75" t="s">
-        <v>32</v>
-      </c>
-      <c r="H75" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>44101500</v>
       </c>
       <c r="B76" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C76" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D76" t="e">
-        <f>VLOOKUP(B76,G$2:H$175,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G76" t="s">
-        <v>34</v>
-      </c>
-      <c r="H76" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>46171500</v>
       </c>
       <c r="B77" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" t="s">
+        <v>164</v>
+      </c>
+      <c r="D77" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E77" xr:uid="{1B28CA15-B4B5-4018-AF0A-6175CA13693E}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="FR0000"/>
+        <filter val="IF0BM0"/>
+        <filter val="IF0CDC"/>
+        <filter val="IF0CK0"/>
+        <filter val="IF0CS0"/>
+        <filter val="IF0CSF"/>
+        <filter val="IF0CT0"/>
+        <filter val="IF0CX0"/>
+        <filter val="IF0CZ0"/>
+        <filter val="IF0LI0"/>
+        <filter val="IF0SB0"/>
+        <filter val="IF0SE0"/>
+        <filter val="IF0SJ0"/>
+        <filter val="IF0ZC0"/>
+        <filter val="IF0ZRX"/>
+        <filter val="IF0ZWX"/>
+        <filter val="JM0A00"/>
+        <filter val="JM0AC0"/>
+        <filter val="JM0GL0"/>
+        <filter val="JM0L00"/>
+        <filter val="JM0LCM"/>
+        <filter val="JM0LF0"/>
+        <filter val="JM0N00"/>
+        <filter val="JM0P00"/>
+        <filter val="JM0PN0"/>
+        <filter val="JM0PP0"/>
+        <filter val="JM0T00"/>
+        <filter val="JM0TP0"/>
+        <filter val="JM0X00"/>
+        <filter val="JT0TEL"/>
+        <filter val="KS0B00"/>
+        <filter val="KS0K00"/>
+        <filter val="MD0MD0"/>
+        <filter val="PU0000"/>
+        <filter val="TP0000"/>
+        <filter val="VA0PAQ"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F526A16-F2FE-4C25-9817-21FBBFBEDD7F}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>46171500</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="5">
+        <v>43360.557515011576</v>
+      </c>
+      <c r="F2" s="5">
+        <v>43360.557515011576</v>
+      </c>
+      <c r="G2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>46171500</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="5">
+        <v>43360.599181678197</v>
+      </c>
+      <c r="F3" s="5">
+        <v>43360.599181678197</v>
+      </c>
+      <c r="G3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>46171500</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="5">
+        <v>43360.640848344898</v>
+      </c>
+      <c r="F4" s="5">
+        <v>43360.640848344898</v>
+      </c>
+      <c r="G4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>46171500</v>
+      </c>
+      <c r="B5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43360.682515011598</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43360.682515011598</v>
+      </c>
+      <c r="G5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>46171500</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="5">
+        <v>43360.724181678197</v>
+      </c>
+      <c r="F6" s="5">
+        <v>43360.724181678197</v>
+      </c>
+      <c r="G6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>46171500</v>
+      </c>
+      <c r="B7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43360.765848344898</v>
+      </c>
+      <c r="F7" s="5">
+        <v>43360.765848344898</v>
+      </c>
+      <c r="G7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>46171500</v>
+      </c>
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="5">
+        <v>43360.807515011598</v>
+      </c>
+      <c r="F8" s="5">
+        <v>43360.807515011598</v>
+      </c>
+      <c r="G8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>46171500</v>
+      </c>
+      <c r="B9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43360.849181678197</v>
+      </c>
+      <c r="F9" s="5">
+        <v>43360.849181678197</v>
+      </c>
+      <c r="G9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>46171501</v>
+      </c>
+      <c r="B10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43360.890848344898</v>
+      </c>
+      <c r="F10" s="5">
+        <v>43360.890848344898</v>
+      </c>
+      <c r="G10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>46171501</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43360.932515011598</v>
+      </c>
+      <c r="F11" s="5">
+        <v>43360.932515011598</v>
+      </c>
+      <c r="G11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>46171501</v>
+      </c>
+      <c r="B12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="5">
+        <v>43360.974181678197</v>
+      </c>
+      <c r="F12" s="5">
+        <v>43360.974181678197</v>
+      </c>
+      <c r="G12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>46171501</v>
+      </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="5">
+        <v>43361.015848344898</v>
+      </c>
+      <c r="F13" s="5">
+        <v>43361.015848344898</v>
+      </c>
+      <c r="G13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>46171501</v>
+      </c>
+      <c r="B14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="5">
+        <v>43361.057515011598</v>
+      </c>
+      <c r="F14" s="5">
+        <v>43361.057515011598</v>
+      </c>
+      <c r="G14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>46171501</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="5">
+        <v>43361.099181678197</v>
+      </c>
+      <c r="F15" s="5">
+        <v>43361.099181678197</v>
+      </c>
+      <c r="G15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>46171505</v>
+      </c>
+      <c r="B16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="5">
+        <v>43361.140848344898</v>
+      </c>
+      <c r="F16" s="5">
+        <v>43361.140848344898</v>
+      </c>
+      <c r="G16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>46171505</v>
+      </c>
+      <c r="B17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>43361.182515011598</v>
+      </c>
+      <c r="F17" s="5">
+        <v>43361.182515011598</v>
+      </c>
+      <c r="G17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>46171505</v>
+      </c>
+      <c r="B18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="5">
+        <v>43361.224181678197</v>
+      </c>
+      <c r="F18" s="5">
+        <v>43361.224181678197</v>
+      </c>
+      <c r="G18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>46171505</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="5">
+        <v>43361.265848344898</v>
+      </c>
+      <c r="F19" s="5">
+        <v>43361.265848344898</v>
+      </c>
+      <c r="G19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>46171505</v>
+      </c>
+      <c r="B20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="5">
+        <v>43361.307515011598</v>
+      </c>
+      <c r="F20" s="5">
+        <v>43361.307515011598</v>
+      </c>
+      <c r="G20" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>46171505</v>
+      </c>
+      <c r="B21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="5">
+        <v>43361.349181678197</v>
+      </c>
+      <c r="F21" s="5">
+        <v>43361.349181678197</v>
+      </c>
+      <c r="G21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>46171505</v>
+      </c>
+      <c r="B22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="5">
+        <v>43361.390848344898</v>
+      </c>
+      <c r="F22" s="5">
+        <v>43361.390848344898</v>
+      </c>
+      <c r="G22" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>46171505</v>
+      </c>
+      <c r="B23" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="5">
+        <v>43361.432515011598</v>
+      </c>
+      <c r="F23" s="5">
+        <v>43361.432515011598</v>
+      </c>
+      <c r="G23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>46171505</v>
+      </c>
+      <c r="B24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="5">
+        <v>43361.474181678197</v>
+      </c>
+      <c r="F24" s="5">
+        <v>43361.474181678197</v>
+      </c>
+      <c r="G24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>46171505</v>
+      </c>
+      <c r="B25" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="5">
+        <v>43361.515848344898</v>
+      </c>
+      <c r="F25" s="5">
+        <v>43361.515848344898</v>
+      </c>
+      <c r="G25" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>46171505</v>
+      </c>
+      <c r="B26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="5">
+        <v>43361.557515011598</v>
+      </c>
+      <c r="F26" s="5">
+        <v>43361.557515011598</v>
+      </c>
+      <c r="G26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>46171505</v>
+      </c>
+      <c r="B27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="5">
+        <v>43361.599181678197</v>
+      </c>
+      <c r="F27" s="5">
+        <v>43361.599181678197</v>
+      </c>
+      <c r="G27" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>46171505</v>
+      </c>
+      <c r="B28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="5">
+        <v>43361.640848344898</v>
+      </c>
+      <c r="F28" s="5">
+        <v>43361.640848344898</v>
+      </c>
+      <c r="G28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>46171505</v>
+      </c>
+      <c r="B29" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="5">
+        <v>43361.682515011598</v>
+      </c>
+      <c r="F29" s="5">
+        <v>43361.682515011598</v>
+      </c>
+      <c r="G29" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>46171514</v>
+      </c>
+      <c r="B30" t="s">
         <v>167</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C30" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="5">
+        <v>43361.724181678197</v>
+      </c>
+      <c r="F30" s="5">
+        <v>43361.724181678197</v>
+      </c>
+      <c r="G30" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>52161525</v>
+      </c>
+      <c r="B31" t="s">
         <v>168</v>
       </c>
-      <c r="D77" t="e">
-        <f>VLOOKUP(B77,G$2:H$175,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G77" t="s">
-        <v>36</v>
-      </c>
-      <c r="H77" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G78" t="s">
-        <v>38</v>
-      </c>
-      <c r="H78" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G79" t="s">
-        <v>40</v>
-      </c>
-      <c r="H79" t="s">
+      <c r="C31" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D31" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G80" t="s">
-        <v>42</v>
-      </c>
-      <c r="H80" t="s">
+      <c r="E31" s="5">
+        <v>43361.765848344898</v>
+      </c>
+      <c r="F31" s="5">
+        <v>43361.765848344898</v>
+      </c>
+      <c r="G31" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32111604</v>
+      </c>
+      <c r="B32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="5">
+        <v>43361.807515011598</v>
+      </c>
+      <c r="F32" s="5">
+        <v>43361.807515011598</v>
+      </c>
+      <c r="G32" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31261501</v>
+      </c>
+      <c r="B33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D33" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G81" t="s">
-        <v>44</v>
-      </c>
-      <c r="H81" t="s">
+      <c r="E33" s="5">
+        <v>43361.849181678197</v>
+      </c>
+      <c r="F33" s="5">
+        <v>43361.849181678197</v>
+      </c>
+      <c r="G33" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31261501</v>
+      </c>
+      <c r="B34" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D34" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G82" t="s">
-        <v>99</v>
-      </c>
-      <c r="H82" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G83" t="s">
-        <v>101</v>
-      </c>
-      <c r="H83" t="s">
+      <c r="E34" s="5">
+        <v>43361.890848344898</v>
+      </c>
+      <c r="F34" s="5">
+        <v>43361.890848344898</v>
+      </c>
+      <c r="G34" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>44101500</v>
+      </c>
+      <c r="B35" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D35" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G84" t="s">
-        <v>16</v>
-      </c>
-      <c r="H84" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G85" t="s">
+      <c r="E35" s="5">
+        <v>43361.932515011598</v>
+      </c>
+      <c r="F35" s="5">
+        <v>43361.932515011598</v>
+      </c>
+      <c r="G35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>82101500</v>
+      </c>
+      <c r="B36" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="5">
+        <v>43361.974181678197</v>
+      </c>
+      <c r="F36" s="5">
+        <v>43361.974181678197</v>
+      </c>
+      <c r="G36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>44101500</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D37" t="s">
         <v>102</v>
       </c>
-      <c r="H85" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G86" t="s">
-        <v>8</v>
-      </c>
-      <c r="H86" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G87" t="s">
-        <v>16</v>
-      </c>
-      <c r="H87" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G88" t="s">
-        <v>12</v>
-      </c>
-      <c r="H88" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="89" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G89" t="s">
-        <v>27</v>
-      </c>
-      <c r="H89" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="90" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G90" t="s">
-        <v>34</v>
-      </c>
-      <c r="H90" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="91" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G91" t="s">
-        <v>54</v>
-      </c>
-      <c r="H91" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="92" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G92" t="s">
-        <v>16</v>
-      </c>
-      <c r="H92" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="93" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G93" t="s">
-        <v>57</v>
-      </c>
-      <c r="H93" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="94" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G94" t="s">
-        <v>59</v>
-      </c>
-      <c r="H94" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="95" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G95" t="s">
-        <v>104</v>
-      </c>
-      <c r="H95" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="96" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G96" t="s">
-        <v>106</v>
-      </c>
-      <c r="H96" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="97" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G97" t="s">
-        <v>108</v>
-      </c>
-      <c r="H97" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="98" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G98" t="s">
-        <v>110</v>
-      </c>
-      <c r="H98" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="99" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G99" t="s">
-        <v>112</v>
-      </c>
-      <c r="H99" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="100" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G100" t="s">
-        <v>114</v>
-      </c>
-      <c r="H100" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="101" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G101" t="s">
-        <v>104</v>
-      </c>
-      <c r="H101" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="102" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G102" t="s">
-        <v>2</v>
-      </c>
-      <c r="H102" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G103" t="s">
-        <v>2</v>
-      </c>
-      <c r="H103" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G104" t="s">
-        <v>116</v>
-      </c>
-      <c r="H104" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="105" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G105" t="s">
-        <v>118</v>
-      </c>
-      <c r="H105" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="106" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G106" t="s">
-        <v>120</v>
-      </c>
-      <c r="H106" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="107" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G107" t="s">
-        <v>4</v>
-      </c>
-      <c r="H107" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="108" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G108" t="s">
-        <v>6</v>
-      </c>
-      <c r="H108" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="109" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G109" t="s">
-        <v>8</v>
-      </c>
-      <c r="H109" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G110" t="s">
-        <v>10</v>
-      </c>
-      <c r="H110" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="111" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G111" t="s">
-        <v>12</v>
-      </c>
-      <c r="H111" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="112" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G112" t="s">
-        <v>14</v>
-      </c>
-      <c r="H112" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="113" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G113" t="s">
-        <v>16</v>
-      </c>
-      <c r="H113" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="114" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G114" t="s">
-        <v>18</v>
-      </c>
-      <c r="H114" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="115" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G115" t="s">
-        <v>20</v>
-      </c>
-      <c r="H115" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="116" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G116" t="s">
-        <v>8</v>
-      </c>
-      <c r="H116" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="117" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G117" t="s">
-        <v>10</v>
-      </c>
-      <c r="H117" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="118" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G118" t="s">
-        <v>12</v>
-      </c>
-      <c r="H118" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="119" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G119" t="s">
-        <v>25</v>
-      </c>
-      <c r="H119" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="120" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G120" t="s">
-        <v>27</v>
-      </c>
-      <c r="H120" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="121" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G121" t="s">
-        <v>8</v>
-      </c>
-      <c r="H121" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="122" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G122" t="s">
-        <v>10</v>
-      </c>
-      <c r="H122" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="123" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G123" t="s">
-        <v>12</v>
-      </c>
-      <c r="H123" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="124" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G124" t="s">
-        <v>32</v>
-      </c>
-      <c r="H124" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="125" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G125" t="s">
-        <v>34</v>
-      </c>
-      <c r="H125" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="126" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G126" t="s">
-        <v>36</v>
-      </c>
-      <c r="H126" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="127" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G127" t="s">
-        <v>38</v>
-      </c>
-      <c r="H127" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="128" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G128" t="s">
-        <v>44</v>
-      </c>
-      <c r="H128" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="129" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G129" t="s">
-        <v>16</v>
-      </c>
-      <c r="H129" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="130" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G130" t="s">
-        <v>47</v>
-      </c>
-      <c r="H130" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="131" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G131" t="s">
-        <v>8</v>
-      </c>
-      <c r="H131" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="132" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G132" t="s">
-        <v>16</v>
-      </c>
-      <c r="H132" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="133" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G133" t="s">
-        <v>12</v>
-      </c>
-      <c r="H133" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="134" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G134" t="s">
-        <v>27</v>
-      </c>
-      <c r="H134" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="135" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G135" t="s">
-        <v>34</v>
-      </c>
-      <c r="H135" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="136" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G136" t="s">
-        <v>16</v>
-      </c>
-      <c r="H136" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="137" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G137" t="s">
-        <v>57</v>
-      </c>
-      <c r="H137" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="138" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G138" t="s">
-        <v>4</v>
-      </c>
-      <c r="H138" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="139" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G139" t="s">
-        <v>6</v>
-      </c>
-      <c r="H139" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="140" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G140" t="s">
-        <v>121</v>
-      </c>
-      <c r="H140" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="141" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G141" t="s">
-        <v>122</v>
-      </c>
-      <c r="H141" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="142" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G142" t="s">
-        <v>123</v>
-      </c>
-      <c r="H142" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="143" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G143" t="s">
-        <v>14</v>
-      </c>
-      <c r="H143" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="144" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G144" t="s">
-        <v>16</v>
-      </c>
-      <c r="H144" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="145" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G145" t="s">
-        <v>18</v>
-      </c>
-      <c r="H145" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="146" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G146" t="s">
-        <v>20</v>
-      </c>
-      <c r="H146" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="147" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G147" t="s">
-        <v>124</v>
-      </c>
-      <c r="H147" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="148" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G148" t="s">
-        <v>125</v>
-      </c>
-      <c r="H148" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="149" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G149" t="s">
-        <v>126</v>
-      </c>
-      <c r="H149" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="150" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G150" t="s">
-        <v>25</v>
-      </c>
-      <c r="H150" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="151" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G151" t="s">
-        <v>27</v>
-      </c>
-      <c r="H151" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="152" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G152" t="s">
-        <v>8</v>
-      </c>
-      <c r="H152" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="153" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G153" t="s">
-        <v>10</v>
-      </c>
-      <c r="H153" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="154" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G154" t="s">
-        <v>12</v>
-      </c>
-      <c r="H154" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="155" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G155" t="s">
-        <v>32</v>
-      </c>
-      <c r="H155" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="156" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G156" t="s">
-        <v>34</v>
-      </c>
-      <c r="H156" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="157" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G157" t="s">
-        <v>36</v>
-      </c>
-      <c r="H157" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="158" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G158" t="s">
-        <v>38</v>
-      </c>
-      <c r="H158" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="159" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G159" t="s">
-        <v>42</v>
-      </c>
-      <c r="H159" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="160" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G160" t="s">
-        <v>44</v>
-      </c>
-      <c r="H160" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="161" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G161" t="s">
-        <v>127</v>
-      </c>
-      <c r="H161" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="162" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G162" t="s">
-        <v>47</v>
-      </c>
-      <c r="H162" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="163" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G163" t="s">
-        <v>128</v>
-      </c>
-      <c r="H163" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="164" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G164" t="s">
-        <v>129</v>
-      </c>
-      <c r="H164" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="165" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G165" t="s">
-        <v>130</v>
-      </c>
-      <c r="H165" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="166" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G166" t="s">
-        <v>131</v>
-      </c>
-      <c r="H166" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="167" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G167" t="s">
-        <v>132</v>
-      </c>
-      <c r="H167" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="168" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G168" t="s">
-        <v>133</v>
-      </c>
-      <c r="H168" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="169" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G169" t="s">
-        <v>57</v>
-      </c>
-      <c r="H169" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="170" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G170" t="s">
-        <v>134</v>
-      </c>
-      <c r="H170" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="171" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G171" t="s">
-        <v>135</v>
-      </c>
-      <c r="H171" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="172" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G172" t="s">
-        <v>136</v>
-      </c>
-      <c r="H172" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="173" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G173" t="s">
-        <v>134</v>
-      </c>
-      <c r="H173" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="174" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G174" t="s">
-        <v>135</v>
-      </c>
-      <c r="H174" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="175" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G175" t="s">
-        <v>136</v>
-      </c>
-      <c r="H175" t="s">
-        <v>119</v>
+      <c r="E37" s="5">
+        <v>43362.015848344898</v>
+      </c>
+      <c r="F37" s="5">
+        <v>43362.015848344898</v>
+      </c>
+      <c r="G37" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -3754,7 +3844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBC4156-EF9C-4681-8DFD-8F199C16975B}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -3770,82 +3860,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3856,7 +3946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629868A6-926C-48A3-951A-50A7BC8A1C2E}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -3870,42 +3960,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3913,15 +4003,15 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3929,7 +4019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A279A96F-D51B-4C97-99F4-C87DF3008974}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3945,34 +4035,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3980,7 +4070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA29286A-D4D2-43ED-928D-526B74FD4119}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3994,26 +4084,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>